<commit_message>
Add New Table Template and Update Table Field
</commit_message>
<xml_diff>
--- a/ProjectDetails.xlsx
+++ b/ProjectDetails.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="183">
   <si>
     <t>Admin Features</t>
   </si>
@@ -273,9 +273,6 @@
     <t>CategoryId</t>
   </si>
   <si>
-    <t>customerId</t>
-  </si>
-  <si>
     <t>ProductId</t>
   </si>
   <si>
@@ -300,12 +297,6 @@
     <t>3/ Orders</t>
   </si>
   <si>
-    <t>5/ product categories</t>
-  </si>
-  <si>
-    <t>CreateDate</t>
-  </si>
-  <si>
     <t>DateTime</t>
   </si>
   <si>
@@ -444,9 +435,6 @@
     <t>SaleEndDate</t>
   </si>
   <si>
-    <t>Brand</t>
-  </si>
-  <si>
     <t>Varchar 30</t>
   </si>
   <si>
@@ -471,18 +459,12 @@
     <t>Customer Activate Date</t>
   </si>
   <si>
-    <t>Mesurment</t>
-  </si>
-  <si>
     <t>Kg, Size,,Ltr etc</t>
   </si>
   <si>
     <t>Mesurment Value</t>
   </si>
   <si>
-    <t xml:space="preserve">EMail </t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -532,6 +514,57 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t>5/ ProductCategories</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Frontent</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>BrandId</t>
+  </si>
+  <si>
+    <t>Brand (Id)</t>
+  </si>
+  <si>
+    <t>CreatDate</t>
+  </si>
+  <si>
+    <t>DeliveryAddress</t>
+  </si>
+  <si>
+    <t>User Creat Date</t>
+  </si>
+  <si>
+    <t>User Update Date</t>
+  </si>
+  <si>
+    <t>9/Brands</t>
+  </si>
+  <si>
+    <t>Measurment</t>
+  </si>
+  <si>
+    <t>10/ProductMapping</t>
+  </si>
+  <si>
+    <t>SaleId</t>
+  </si>
+  <si>
+    <t>Sale (Id)</t>
   </si>
 </sst>
 </file>
@@ -1184,6 +1217,9 @@
       <c r="C20" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="F20" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="21" spans="1:14" ht="23.25">
       <c r="C21" s="8" t="s">
@@ -1198,20 +1234,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N90"/>
+  <dimension ref="B2:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N107" sqref="N107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="28.5">
+    <row r="2" spans="2:12" ht="28.5">
       <c r="B2" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="26.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="26.25">
       <c r="B4" s="15" t="s">
         <v>25</v>
       </c>
@@ -1232,14 +1272,13 @@
         <v>28</v>
       </c>
       <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>29</v>
       </c>
+      <c r="K4" s="17"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" spans="2:13" ht="18.75">
+    </row>
+    <row r="5" spans="2:12" ht="18.75">
       <c r="B5" s="27" t="s">
         <v>30</v>
       </c>
@@ -1265,15 +1304,14 @@
         <v>35</v>
       </c>
       <c r="L5" s="23"/>
-      <c r="M5" s="27"/>
-    </row>
-    <row r="6" spans="2:13" ht="18.75">
+    </row>
+    <row r="6" spans="2:12" ht="18.75">
       <c r="B6" s="27" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>43</v>
@@ -1285,7 +1323,7 @@
         <v>35</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -1293,15 +1331,14 @@
         <v>35</v>
       </c>
       <c r="L6" s="23"/>
-      <c r="M6" s="27"/>
-    </row>
-    <row r="7" spans="2:13" ht="18.75">
+    </row>
+    <row r="7" spans="2:12" ht="18.75">
       <c r="B7" s="27" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="28" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>43</v>
@@ -1321,15 +1358,14 @@
         <v>35</v>
       </c>
       <c r="L7" s="23"/>
-      <c r="M7" s="27"/>
-    </row>
-    <row r="8" spans="2:13" ht="18.75">
+    </row>
+    <row r="8" spans="2:12" ht="18.75">
       <c r="B8" s="27" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>43</v>
@@ -1349,15 +1385,14 @@
         <v>35</v>
       </c>
       <c r="L8" s="23"/>
-      <c r="M8" s="27"/>
-    </row>
-    <row r="9" spans="2:13" ht="18.75">
+    </row>
+    <row r="9" spans="2:12" ht="18.75">
       <c r="B9" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>43</v>
@@ -1369,7 +1404,7 @@
         <v>34</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
@@ -1377,15 +1412,14 @@
         <v>35</v>
       </c>
       <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="10" spans="2:13" ht="18.75">
+    </row>
+    <row r="10" spans="2:12" ht="18.75">
       <c r="B10" s="27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="28" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>43</v>
@@ -1397,7 +1431,7 @@
         <v>34</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
@@ -1405,9 +1439,8 @@
         <v>35</v>
       </c>
       <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-    </row>
-    <row r="11" spans="2:13" ht="18.75">
+    </row>
+    <row r="11" spans="2:12" ht="18.75">
       <c r="B11" s="27" t="s">
         <v>41</v>
       </c>
@@ -1433,15 +1466,14 @@
         <v>35</v>
       </c>
       <c r="L11" s="23"/>
-      <c r="M11" s="27"/>
-    </row>
-    <row r="12" spans="2:13" ht="18.75">
+    </row>
+    <row r="12" spans="2:12" ht="18.75">
       <c r="B12" s="27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>43</v>
@@ -1453,7 +1485,7 @@
         <v>34</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
@@ -1461,9 +1493,8 @@
         <v>35</v>
       </c>
       <c r="L12" s="23"/>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="13" spans="2:13" ht="18.75">
+    </row>
+    <row r="13" spans="2:12" ht="18.75">
       <c r="B13" s="27" t="s">
         <v>44</v>
       </c>
@@ -1489,15 +1520,14 @@
         <v>35</v>
       </c>
       <c r="L13" s="23"/>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" spans="2:13" ht="18.75">
+    </row>
+    <row r="14" spans="2:12" ht="18.75">
       <c r="B14" s="27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="28" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E14" s="27" t="s">
         <v>43</v>
@@ -1509,7 +1539,7 @@
         <v>34</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
@@ -1517,15 +1547,14 @@
         <v>35</v>
       </c>
       <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-    </row>
-    <row r="15" spans="2:13" ht="18.75">
+    </row>
+    <row r="15" spans="2:12" ht="18.75">
       <c r="B15" s="27" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E15" s="27" t="s">
         <v>43</v>
@@ -1537,7 +1566,7 @@
         <v>34</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -1545,15 +1574,14 @@
         <v>35</v>
       </c>
       <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-    </row>
-    <row r="16" spans="2:13" ht="18.75">
+    </row>
+    <row r="16" spans="2:12" ht="18.75">
       <c r="B16" s="27" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E16" s="27" t="s">
         <v>43</v>
@@ -1565,7 +1593,7 @@
         <v>34</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
@@ -1573,15 +1601,14 @@
         <v>35</v>
       </c>
       <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-    </row>
-    <row r="17" spans="2:13" ht="18.75">
+    </row>
+    <row r="17" spans="2:12" ht="18.75">
       <c r="B17" s="27" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="28" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E17" s="27" t="s">
         <v>43</v>
@@ -1593,7 +1620,7 @@
         <v>34</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -1601,14 +1628,13 @@
         <v>35</v>
       </c>
       <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-    </row>
-    <row r="19" spans="2:13" ht="31.5">
+    </row>
+    <row r="19" spans="2:12" ht="31.5">
       <c r="B19" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="26.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="26.25">
       <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
@@ -1635,7 +1661,7 @@
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
     </row>
-    <row r="22" spans="2:13" ht="18.75">
+    <row r="22" spans="2:12" ht="18.75">
       <c r="B22" s="23" t="s">
         <v>30</v>
       </c>
@@ -1662,7 +1688,7 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
     </row>
-    <row r="23" spans="2:13" ht="18.75">
+    <row r="23" spans="2:12" ht="18.75">
       <c r="B23" s="23" t="s">
         <v>50</v>
       </c>
@@ -1689,7 +1715,7 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
     </row>
-    <row r="24" spans="2:13" ht="18.75">
+    <row r="24" spans="2:12" ht="18.75">
       <c r="B24" s="23" t="s">
         <v>33</v>
       </c>
@@ -1716,7 +1742,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
     </row>
-    <row r="25" spans="2:13" ht="18.75">
+    <row r="25" spans="2:12" ht="18.75">
       <c r="B25" s="23" t="s">
         <v>84</v>
       </c>
@@ -1743,7 +1769,7 @@
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
     </row>
-    <row r="26" spans="2:13" ht="18.75">
+    <row r="26" spans="2:12" ht="18.75">
       <c r="B26" s="23" t="s">
         <v>28</v>
       </c>
@@ -1770,7 +1796,7 @@
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
     </row>
-    <row r="27" spans="2:13" ht="18.75">
+    <row r="27" spans="2:12" ht="18.75">
       <c r="B27" s="23" t="s">
         <v>61</v>
       </c>
@@ -1797,7 +1823,7 @@
       <c r="K27" s="23"/>
       <c r="L27" s="23"/>
     </row>
-    <row r="28" spans="2:13" ht="18.75">
+    <row r="28" spans="2:12" ht="18.75">
       <c r="B28" s="23" t="s">
         <v>64</v>
       </c>
@@ -1824,13 +1850,13 @@
       <c r="K28" s="23"/>
       <c r="L28" s="23"/>
     </row>
-    <row r="29" spans="2:13" ht="18.75">
+    <row r="29" spans="2:12" ht="18.75">
       <c r="B29" s="23" t="s">
-        <v>95</v>
+        <v>174</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>43</v>
@@ -1842,7 +1868,7 @@
         <v>34</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I29" s="24"/>
       <c r="J29" s="23" t="s">
@@ -1851,7 +1877,7 @@
       <c r="K29" s="23"/>
       <c r="L29" s="23"/>
     </row>
-    <row r="30" spans="2:13" ht="18.75">
+    <row r="30" spans="2:12" ht="18.75">
       <c r="B30" s="23" t="s">
         <v>67</v>
       </c>
@@ -1878,13 +1904,13 @@
       <c r="K30" s="23"/>
       <c r="L30" s="23"/>
     </row>
-    <row r="31" spans="2:13" ht="18.75">
+    <row r="31" spans="2:12" ht="18.75">
       <c r="B31" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>43</v>
@@ -1896,7 +1922,7 @@
         <v>34</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I31" s="24"/>
       <c r="J31" s="23" t="s">
@@ -1905,13 +1931,13 @@
       <c r="K31" s="23"/>
       <c r="L31" s="23"/>
     </row>
-    <row r="32" spans="2:13" ht="18.75">
+    <row r="32" spans="2:12" ht="18.75">
       <c r="B32" s="23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E32" s="23" t="s">
         <v>43</v>
@@ -1923,7 +1949,7 @@
         <v>34</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I32" s="24"/>
       <c r="J32" s="23" t="s">
@@ -1934,11 +1960,11 @@
     </row>
     <row r="33" spans="2:14" ht="18.75">
       <c r="B33" s="23" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E33" s="23" t="s">
         <v>43</v>
@@ -1950,7 +1976,7 @@
         <v>34</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I33" s="24"/>
       <c r="J33" s="23" t="s">
@@ -1961,11 +1987,11 @@
     </row>
     <row r="34" spans="2:14" ht="18.75">
       <c r="B34" s="23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E34" s="23" t="s">
         <v>43</v>
@@ -1977,7 +2003,7 @@
         <v>34</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I34" s="24"/>
       <c r="J34" s="23" t="s">
@@ -1988,11 +2014,11 @@
     </row>
     <row r="35" spans="2:14" ht="18.75">
       <c r="B35" s="23" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="24" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E35" s="23" t="s">
         <v>43</v>
@@ -2000,22 +2026,27 @@
       <c r="F35" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="23" t="s">
-        <v>34</v>
+      <c r="G35" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I35" s="24"/>
       <c r="J35" s="23" t="s">
-        <v>34</v>
+        <v>173</v>
       </c>
       <c r="K35" s="23"/>
       <c r="L35" s="23"/>
     </row>
     <row r="37" spans="2:14" ht="31.5">
       <c r="B37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="M38" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="2:14" ht="26.25">
@@ -2074,7 +2105,7 @@
     </row>
     <row r="41" spans="2:14" ht="18.75">
       <c r="B41" s="23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="24" t="s">
@@ -2099,7 +2130,7 @@
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
       <c r="N41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="2:14" ht="18.75">
@@ -2120,7 +2151,7 @@
         <v>34</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I42" s="24"/>
       <c r="J42" s="23" t="s">
@@ -2131,7 +2162,7 @@
     </row>
     <row r="43" spans="2:14" ht="18.75">
       <c r="B43" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="24" t="s">
@@ -2147,7 +2178,7 @@
         <v>34</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I43" s="24"/>
       <c r="J43" s="23" t="s">
@@ -2158,7 +2189,7 @@
     </row>
     <row r="44" spans="2:14" ht="18.75">
       <c r="B44" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="24" t="s">
@@ -2185,11 +2216,11 @@
     </row>
     <row r="45" spans="2:14" ht="18.75">
       <c r="B45" s="23" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E45" s="23" t="s">
         <v>43</v>
@@ -2212,23 +2243,23 @@
     </row>
     <row r="46" spans="2:14" ht="18.75">
       <c r="B46" s="23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46" s="24" t="s">
         <v>96</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G46" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H46" s="24" t="s">
-        <v>99</v>
       </c>
       <c r="I46" s="24"/>
       <c r="J46" s="23" t="s">
@@ -2239,11 +2270,11 @@
     </row>
     <row r="47" spans="2:14" ht="18.75">
       <c r="B47" s="23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E47" s="23" t="s">
         <v>43</v>
@@ -2255,7 +2286,7 @@
         <v>34</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I47" s="24"/>
       <c r="J47" s="23" t="s">
@@ -2266,40 +2297,26 @@
     </row>
     <row r="48" spans="2:14" ht="18.75">
       <c r="B48" s="23" t="s">
-        <v>121</v>
+        <v>175</v>
       </c>
       <c r="C48" s="23"/>
-      <c r="D48" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G48" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H48" s="24" t="s">
-        <v>122</v>
-      </c>
+      <c r="D48" s="24"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="24"/>
       <c r="I48" s="24"/>
-      <c r="J48" s="23" t="s">
-        <v>34</v>
-      </c>
+      <c r="J48" s="23"/>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
     </row>
-    <row r="49" spans="2:13" ht="18.75">
+    <row r="49" spans="2:12" ht="18.75">
       <c r="B49" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="23" t="s">
-        <v>44</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C49" s="23"/>
       <c r="D49" s="24" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E49" s="23" t="s">
         <v>43</v>
@@ -2311,24 +2328,22 @@
         <v>34</v>
       </c>
       <c r="H49" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="I49" s="24" t="s">
-        <v>44</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="I49" s="24"/>
       <c r="J49" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
     </row>
-    <row r="50" spans="2:13" ht="18.75">
+    <row r="50" spans="2:12" ht="18.75">
       <c r="B50" s="23" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="24" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="E50" s="23" t="s">
         <v>43</v>
@@ -2340,22 +2355,24 @@
         <v>34</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="I50" s="24"/>
+        <v>99</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>44</v>
+      </c>
       <c r="J50" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K50" s="23"/>
       <c r="L50" s="23"/>
     </row>
-    <row r="51" spans="2:13" ht="18.75">
+    <row r="51" spans="2:12" ht="18.75">
       <c r="B51" s="23" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="24" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="E51" s="23" t="s">
         <v>43</v>
@@ -2367,107 +2384,104 @@
         <v>34</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="I51" s="19"/>
+        <v>145</v>
+      </c>
+      <c r="I51" s="24"/>
       <c r="J51" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" ht="28.5">
-      <c r="B53" s="11" t="s">
+      <c r="K51" s="23"/>
+      <c r="L51" s="23"/>
+    </row>
+    <row r="52" spans="2:12" ht="18.75">
+      <c r="B52" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="23"/>
+      <c r="D52" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G52" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I52" s="19"/>
+      <c r="J52" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+    </row>
+    <row r="54" spans="2:12" ht="28.5">
+      <c r="B54" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="2:13" ht="26.25">
-      <c r="B55" s="13" t="s">
+    <row r="56" spans="2:12" ht="26.25">
+      <c r="B56" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13" t="s">
+      <c r="C56" s="13"/>
+      <c r="D56" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E56" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G55" s="13" t="s">
+      <c r="F56" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G56" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H55" s="13" t="s">
+      <c r="H56" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13" t="s">
+      <c r="I56" s="13"/>
+      <c r="J56" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K55" s="13"/>
-      <c r="L55" s="14"/>
-    </row>
-    <row r="56" spans="2:13" ht="18.75">
-      <c r="B56" s="23" t="s">
+      <c r="K56" s="13"/>
+      <c r="L56" s="14"/>
+    </row>
+    <row r="57" spans="2:12" ht="18.75">
+      <c r="B57" s="23" t="s">
         <v>30</v>
-      </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E56" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H56" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="I56" s="24"/>
-      <c r="J56" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K56" s="23"/>
-      <c r="L56" s="23"/>
-    </row>
-    <row r="57" spans="2:13" ht="18.75">
-      <c r="B57" s="23" t="s">
-        <v>80</v>
       </c>
       <c r="C57" s="23"/>
       <c r="D57" s="24" t="s">
         <v>40</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F57" s="24" t="s">
         <v>55</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I57" s="24"/>
       <c r="J57" s="23" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="K57" s="23"/>
       <c r="L57" s="23"/>
     </row>
-    <row r="58" spans="2:13" ht="18.75">
+    <row r="58" spans="2:12" ht="18.75">
       <c r="B58" s="23" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C58" s="23"/>
       <c r="D58" s="24" t="s">
@@ -2483,22 +2497,22 @@
         <v>56</v>
       </c>
       <c r="H58" s="24" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="I58" s="24"/>
       <c r="J58" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K58" s="23"/>
       <c r="L58" s="23"/>
     </row>
-    <row r="59" spans="2:13" ht="18.75">
+    <row r="59" spans="2:12" ht="18.75">
       <c r="B59" s="23" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C59" s="23"/>
       <c r="D59" s="24" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="E59" s="23" t="s">
         <v>43</v>
@@ -2506,26 +2520,26 @@
       <c r="F59" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G59" s="23" t="s">
-        <v>34</v>
+      <c r="G59" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H59" s="24" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="I59" s="24"/>
       <c r="J59" s="23" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="K59" s="23"/>
       <c r="L59" s="23"/>
     </row>
-    <row r="60" spans="2:13" ht="18.75">
+    <row r="60" spans="2:12" ht="18.75">
       <c r="B60" s="23" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="C60" s="23"/>
       <c r="D60" s="24" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E60" s="23" t="s">
         <v>43</v>
@@ -2537,7 +2551,7 @@
         <v>34</v>
       </c>
       <c r="H60" s="24" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I60" s="24"/>
       <c r="J60" s="23" t="s">
@@ -2546,87 +2560,87 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
     </row>
-    <row r="61" spans="2:13">
-      <c r="B61" s="12"/>
-    </row>
-    <row r="62" spans="2:13" ht="31.5">
-      <c r="B62" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" ht="26.25">
-      <c r="B64" s="13" t="s">
+    <row r="61" spans="2:12" ht="18.75">
+      <c r="B61" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H61" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I61" s="24"/>
+      <c r="J61" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+    </row>
+    <row r="62" spans="2:12">
+      <c r="B62" s="12"/>
+    </row>
+    <row r="63" spans="2:12" ht="31.5">
+      <c r="B63" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" ht="26.25">
+      <c r="B65" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13" t="s">
+      <c r="C65" s="13"/>
+      <c r="D65" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E64" s="13" t="s">
+      <c r="E65" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F64" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G64" s="13" t="s">
+      <c r="F65" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G65" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H64" s="13" t="s">
+      <c r="H65" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13" t="s">
+      <c r="I65" s="13"/>
+      <c r="J65" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="K64" s="13"/>
-      <c r="L64" s="18"/>
-    </row>
-    <row r="65" spans="2:12" ht="18.75">
-      <c r="B65" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C65" s="23"/>
-      <c r="D65" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E65" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G65" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H65" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I65" s="24"/>
-      <c r="J65" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K65" s="23"/>
-      <c r="L65" s="23"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="18"/>
     </row>
     <row r="66" spans="2:12" ht="18.75">
       <c r="B66" s="23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C66" s="23"/>
       <c r="D66" s="24" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F66" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G66" s="23" t="s">
-        <v>34</v>
+      <c r="G66" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="I66" s="24"/>
       <c r="J66" s="23" t="s">
@@ -2635,126 +2649,126 @@
       <c r="K66" s="23"/>
       <c r="L66" s="23"/>
     </row>
-    <row r="68" spans="2:12" ht="31.5">
-      <c r="B68" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" ht="26.25">
-      <c r="B70" s="13" t="s">
+    <row r="67" spans="2:12" ht="18.75">
+      <c r="B67" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="23"/>
+      <c r="D67" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G67" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="I67" s="24"/>
+      <c r="J67" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K67" s="23"/>
+      <c r="L67" s="23"/>
+    </row>
+    <row r="69" spans="2:12" ht="31.5">
+      <c r="B69" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" ht="26.25">
+      <c r="B71" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13" t="s">
+      <c r="C71" s="13"/>
+      <c r="D71" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E70" s="13" t="s">
+      <c r="E71" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F70" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G70" s="13" t="s">
+      <c r="F71" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H70" s="13" t="s">
+      <c r="H71" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13" t="s">
+      <c r="I71" s="13"/>
+      <c r="J71" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K70" s="13"/>
-      <c r="L70" s="21"/>
-    </row>
-    <row r="71" spans="2:12" ht="18.75">
-      <c r="B71" s="23" t="s">
+      <c r="K71" s="13"/>
+      <c r="L71" s="21"/>
+    </row>
+    <row r="72" spans="2:12" ht="18.75">
+      <c r="B72" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C71" s="23"/>
-      <c r="D71" s="24" t="s">
+      <c r="C72" s="23"/>
+      <c r="D72" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E71" s="23" t="s">
+      <c r="E72" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F71" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G71" s="26" t="s">
+      <c r="F72" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G72" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H71" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="I71" s="24"/>
-      <c r="J71" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K71" s="23"/>
-      <c r="L71" s="23"/>
-    </row>
-    <row r="72" spans="2:12" ht="18.75">
-      <c r="B72" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="C72" s="27"/>
-      <c r="D72" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="E72" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F72" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="G72" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="H72" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="I72" s="28"/>
-      <c r="J72" s="27" t="s">
-        <v>35</v>
+      <c r="H72" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I72" s="24"/>
+      <c r="J72" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="K72" s="23"/>
       <c r="L72" s="23"/>
     </row>
     <row r="73" spans="2:12" ht="18.75">
-      <c r="B73" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="E73" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G73" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H73" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="I73" s="24"/>
-      <c r="J73" s="23" t="s">
-        <v>34</v>
+      <c r="B73" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73" s="27"/>
+      <c r="D73" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E73" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G73" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H73" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I73" s="28"/>
+      <c r="J73" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="K73" s="23"/>
       <c r="L73" s="23"/>
     </row>
     <row r="74" spans="2:12" ht="18.75">
       <c r="B74" s="23" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="C74" s="23"/>
       <c r="D74" s="24" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="E74" s="23" t="s">
         <v>43</v>
@@ -2762,26 +2776,26 @@
       <c r="F74" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G74" s="26" t="s">
-        <v>56</v>
+      <c r="G74" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="I74" s="24"/>
       <c r="J74" s="23" t="s">
-        <v>106</v>
+        <v>34</v>
       </c>
       <c r="K74" s="23"/>
       <c r="L74" s="23"/>
     </row>
     <row r="75" spans="2:12" ht="18.75">
       <c r="B75" s="23" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C75" s="23"/>
       <c r="D75" s="24" t="s">
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="E75" s="23" t="s">
         <v>43</v>
@@ -2789,264 +2803,264 @@
       <c r="F75" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G75" s="23" t="s">
-        <v>34</v>
+      <c r="G75" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="I75" s="24"/>
       <c r="J75" s="23" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="K75" s="23"/>
       <c r="L75" s="23"/>
     </row>
     <row r="76" spans="2:12" ht="18.75">
       <c r="B76" s="23" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="C76" s="23"/>
       <c r="D76" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G76" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H76" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="E76" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G76" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H76" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="I76" s="19"/>
+      <c r="I76" s="24"/>
       <c r="J76" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K76" s="20"/>
-      <c r="L76" s="20"/>
-    </row>
-    <row r="78" spans="2:12" ht="31.5">
-      <c r="B78" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="2:12" ht="26.25">
-      <c r="B80" s="13" t="s">
+      <c r="K76" s="23"/>
+      <c r="L76" s="23"/>
+    </row>
+    <row r="77" spans="2:12" ht="18.75">
+      <c r="B77" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C77" s="23"/>
+      <c r="D77" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E77" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G77" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H77" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="I77" s="24"/>
+      <c r="J77" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K77" s="23"/>
+      <c r="L77" s="23"/>
+    </row>
+    <row r="78" spans="2:12" ht="18.75">
+      <c r="B78" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C78" s="20"/>
+      <c r="D78" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E78" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G78" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H78" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="I78" s="19"/>
+      <c r="J78" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K78" s="23"/>
+      <c r="L78" s="23"/>
+    </row>
+    <row r="79" spans="2:12" ht="18.75">
+      <c r="B79" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" s="23"/>
+      <c r="D79" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E79" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H79" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I79" s="19"/>
+      <c r="J79" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K79" s="20"/>
+      <c r="L79" s="20"/>
+    </row>
+    <row r="81" spans="2:12" ht="31.5">
+      <c r="B81" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" ht="26.25">
+      <c r="B83" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13" t="s">
+      <c r="C83" s="13"/>
+      <c r="D83" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E80" s="13" t="s">
+      <c r="E83" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F80" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G80" s="13" t="s">
+      <c r="F83" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G83" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H80" s="13" t="s">
+      <c r="H83" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13" t="s">
+      <c r="I83" s="13"/>
+      <c r="J83" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K80" s="13"/>
-      <c r="L80" s="21"/>
-    </row>
-    <row r="81" spans="2:12" ht="18.75">
-      <c r="B81" s="23" t="s">
+      <c r="K83" s="13"/>
+      <c r="L83" s="21"/>
+    </row>
+    <row r="84" spans="2:12" ht="18.75">
+      <c r="B84" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="23"/>
-      <c r="D81" s="24" t="s">
+      <c r="C84" s="23"/>
+      <c r="D84" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E81" s="23" t="s">
+      <c r="E84" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F81" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G81" s="26" t="s">
+      <c r="F84" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G84" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H81" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="I81" s="24"/>
-      <c r="J81" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K81" s="23"/>
-      <c r="L81" s="23"/>
-    </row>
-    <row r="82" spans="2:12" ht="18.75">
-      <c r="B82" s="23" t="s">
+      <c r="H84" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="I84" s="24"/>
+      <c r="J84" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K84" s="23"/>
+      <c r="L84" s="23"/>
+    </row>
+    <row r="85" spans="2:12" ht="18.75">
+      <c r="B85" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C82" s="23"/>
-      <c r="D82" s="24" t="s">
+      <c r="C85" s="23"/>
+      <c r="D85" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E82" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F82" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G82" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H82" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="I82" s="24"/>
-      <c r="J82" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K82" s="23"/>
-      <c r="L82" s="23"/>
-    </row>
-    <row r="84" spans="2:12" ht="31.5">
-      <c r="B84" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="86" spans="2:12" ht="26.25">
-      <c r="B86" s="13" t="s">
+      <c r="E85" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F85" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G85" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H85" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I85" s="24"/>
+      <c r="J85" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K85" s="23"/>
+      <c r="L85" s="23"/>
+    </row>
+    <row r="87" spans="2:12" ht="31.5">
+      <c r="B87" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" ht="26.25">
+      <c r="B89" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13" t="s">
+      <c r="C89" s="13"/>
+      <c r="D89" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E86" s="13" t="s">
+      <c r="E89" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F86" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G86" s="13" t="s">
+      <c r="F89" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G89" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H86" s="13" t="s">
+      <c r="H89" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13" t="s">
+      <c r="I89" s="13"/>
+      <c r="J89" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-    </row>
-    <row r="87" spans="2:12" ht="18.75">
-      <c r="B87" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C87" s="23"/>
-      <c r="D87" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E87" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F87" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G87" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H87" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="I87" s="24"/>
-      <c r="J87" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K87" s="23"/>
-      <c r="L87" s="23"/>
-    </row>
-    <row r="88" spans="2:12" ht="18.75">
-      <c r="B88" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C88" s="23"/>
-      <c r="D88" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E88" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F88" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G88" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H88" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="I88" s="24"/>
-      <c r="J88" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K88" s="23"/>
-      <c r="L88" s="23"/>
-    </row>
-    <row r="89" spans="2:12" ht="18.75">
-      <c r="B89" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C89" s="23"/>
-      <c r="D89" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="E89" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F89" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G89" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H89" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="I89" s="24"/>
-      <c r="J89" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K89" s="23"/>
-      <c r="L89" s="23"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
     </row>
     <row r="90" spans="2:12" ht="18.75">
       <c r="B90" s="23" t="s">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="C90" s="23"/>
       <c r="D90" s="24" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="E90" s="23" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F90" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G90" s="23" t="s">
-        <v>34</v>
+      <c r="G90" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="H90" s="24" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I90" s="24"/>
       <c r="J90" s="23" t="s">
@@ -3054,6 +3068,286 @@
       </c>
       <c r="K90" s="23"/>
       <c r="L90" s="23"/>
+    </row>
+    <row r="91" spans="2:12" ht="18.75">
+      <c r="B91" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C91" s="23"/>
+      <c r="D91" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G91" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H91" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="I91" s="24"/>
+      <c r="J91" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K91" s="23"/>
+      <c r="L91" s="23"/>
+    </row>
+    <row r="92" spans="2:12" ht="18.75">
+      <c r="B92" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92" s="23"/>
+      <c r="D92" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G92" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H92" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="I92" s="24"/>
+      <c r="J92" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K92" s="23"/>
+      <c r="L92" s="23"/>
+    </row>
+    <row r="93" spans="2:12" ht="18.75">
+      <c r="B93" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" s="23"/>
+      <c r="D93" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E93" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F93" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G93" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H93" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="I93" s="24"/>
+      <c r="J93" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K93" s="23"/>
+      <c r="L93" s="23"/>
+    </row>
+    <row r="95" spans="2:12" ht="31.5">
+      <c r="B95" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" ht="26.25">
+      <c r="B97" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G97" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K97" s="13"/>
+      <c r="L97" s="13"/>
+    </row>
+    <row r="98" spans="2:12" ht="18.75">
+      <c r="B98" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C98" s="23"/>
+      <c r="D98" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E98" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F98" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G98" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H98" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I98" s="24"/>
+      <c r="J98" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K98" s="23"/>
+      <c r="L98" s="23"/>
+    </row>
+    <row r="99" spans="2:12" ht="18.75">
+      <c r="B99" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C99" s="23"/>
+      <c r="D99" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F99" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G99" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H99" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="I99" s="24"/>
+      <c r="J99" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K99" s="23"/>
+      <c r="L99" s="23"/>
+    </row>
+    <row r="101" spans="2:12" ht="31.5">
+      <c r="B101" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" ht="26.25">
+      <c r="B103" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G103" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
+    </row>
+    <row r="104" spans="2:12" ht="18.75">
+      <c r="B104" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C104" s="23"/>
+      <c r="D104" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E104" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F104" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G104" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H104" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I104" s="24"/>
+      <c r="J104" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K104" s="23"/>
+      <c r="L104" s="23"/>
+    </row>
+    <row r="105" spans="2:12" ht="18.75">
+      <c r="B105" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C105" s="23"/>
+      <c r="D105" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E105" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F105" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G105" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H105" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I105" s="24"/>
+      <c r="J105" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="K105" s="23"/>
+      <c r="L105" s="23"/>
+    </row>
+    <row r="106" spans="2:12" ht="18.75">
+      <c r="B106" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C106" s="23"/>
+      <c r="D106" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E106" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F106" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G106" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H106" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I106" s="24"/>
+      <c r="J106" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="K106" s="23"/>
+      <c r="L106" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3063,12 +3357,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A4:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="1:5">
+      <c r="E4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>